<commit_message>
Added ACS 1-year 2022 data
</commit_message>
<xml_diff>
--- a/GOAL-1/viz_source_files/Goal1_hh_income.xlsx
+++ b/GOAL-1/viz_source_files/Goal1_hh_income.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jenkir\Desktop\BDC\Baltimore_Together\measuring-success-metrics\BT-equity-metric-analysis\GOAL-1\viz_source_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB08776E-2FFB-4817-AEF8-8EFF1FD6AABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12A1846-ED42-4FCE-AD32-FCA6999BBECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-12" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,6 +423,7 @@
   <cols>
     <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>